<commit_message>
add alot asset and add card bag and achieve random generation for the normal level
</commit_message>
<xml_diff>
--- a/Assets/_Excel/level.xlsx
+++ b/Assets/_Excel/level.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProject\Card\Card-game_test\Assets\_Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC877030-5992-410A-99E3-C56ECDC7E853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D3FB92A-5EE0-4389-890D-9AA956309B6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1670" yWindow="2890" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="3690" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -51,14 +51,13 @@
     <t>10001=10002=10003</t>
   </si>
   <si>
-    <t>2040,852,1728=2040,448,172</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>1616,646,1728=2040,852,1728=2040,448,1728</t>
   </si>
   <si>
     <t>1616,646,1728</t>
+  </si>
+  <si>
+    <t>2040,852,1728=2040,448,1728</t>
   </si>
 </sst>
 </file>
@@ -438,7 +437,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -486,7 +485,7 @@
         <v>10001</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -500,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -514,7 +513,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>